<commit_message>
removed unused light control files
</commit_message>
<xml_diff>
--- a/Vial_board_pin_list_10.18.20.xlsx
+++ b/Vial_board_pin_list_10.18.20.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbord\Dropbox\Cyano\Evolver\git_clones\evolver-arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639289D6-6FAF-4E4F-A32D-3D557BC6A582}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F499B43-FF20-47C0-A105-AECD436251B1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D7B52437-BE9F-4EAE-A44A-B5BC2DEDF0E3}"/>
   </bookViews>
@@ -81,10 +81,10 @@
     <t>Temp</t>
   </si>
   <si>
-    <t>LIGHT_PD_10.17.20</t>
-  </si>
-  <si>
     <t>ODLED_only</t>
+  </si>
+  <si>
+    <t>OD_LIGHT_SWITCHING</t>
   </si>
 </sst>
 </file>
@@ -451,7 +451,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -536,7 +536,7 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -561,7 +561,7 @@
         <v>4</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>